<commit_message>
modificando matris de seguimiento
</commit_message>
<xml_diff>
--- a/documentacion_del_proyecto/Matriz de seguimiento.xlsx
+++ b/documentacion_del_proyecto/Matriz de seguimiento.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cf206\OneDrive\Desktop\scuele\R_Universisdad_Segunda_Mano\documentacion_del_proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\Desktop\proyectos\universidad_segunda\documentacion_del_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1382588A-3CFE-4FD9-AEDC-8BDB91414A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Status</t>
   </si>
@@ -45,9 +44,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Favoritos</t>
-  </si>
-  <si>
     <t>Inicio de sesión</t>
   </si>
   <si>
@@ -69,28 +65,28 @@
     <t>Perfil de usuario</t>
   </si>
   <si>
-    <t>Seccion de anime</t>
-  </si>
-  <si>
     <t>Carro de compras</t>
   </si>
   <si>
     <t>Página de los productos</t>
   </si>
   <si>
-    <t>Seccion de electrónica</t>
-  </si>
-  <si>
     <t>Sin empezar</t>
   </si>
   <si>
     <t>Página Inicial (Index)</t>
+  </si>
+  <si>
+    <t>Misproductos</t>
+  </si>
+  <si>
+    <t>Filtro por secciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,22 +597,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -628,7 +624,7 @@
       <c r="E1" s="12"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="6" t="s">
@@ -641,13 +637,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="1" t="s">
@@ -657,9 +653,9 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
@@ -669,21 +665,21 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
@@ -693,9 +689,9 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
@@ -705,9 +701,9 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="1"/>
@@ -717,21 +713,21 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="1"/>
@@ -741,21 +737,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
@@ -765,21 +761,21 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="1"/>
@@ -789,17 +785,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
matris de segumiento actualizada
</commit_message>
<xml_diff>
--- a/documentacion_del_proyecto/Matriz de seguimiento.xlsx
+++ b/documentacion_del_proyecto/Matriz de seguimiento.xlsx
@@ -601,7 +601,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,10 +766,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Se desarrollan las autenticaciones y cambios en la ortorafía.
</commit_message>
<xml_diff>
--- a/documentacion_del_proyecto/Matriz de seguimiento.xlsx
+++ b/documentacion_del_proyecto/Matriz de seguimiento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\Desktop\proyectos\universidad_segunda\documentacion_del_proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cf206\OneDrive\Desktop\ytabajo_desarrollo_web\universidad_segunda\documentacion_del_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90162AA1-18C8-478E-9B77-073B444E8C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,22 +598,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -624,7 +625,7 @@
       <c r="E1" s="12"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="6" t="s">
@@ -641,7 +642,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -653,7 +654,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -665,31 +666,31 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -701,7 +702,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -713,7 +714,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -725,7 +726,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -737,7 +738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
@@ -749,7 +750,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -761,7 +762,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -773,7 +774,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -785,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="1"/>

</xml_diff>